<commit_message>
added in excel sheet
</commit_message>
<xml_diff>
--- a/ZSolved Problems.xlsx
+++ b/ZSolved Problems.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\LeetCode\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>PROBLEM SOLVED</t>
   </si>
@@ -292,6 +291,15 @@
   </si>
   <si>
     <t>Find smallest letter greater than target</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array/submissions/</t>
+  </si>
+  <si>
+    <t>Find first and last occurrence of the number in an array</t>
   </si>
 </sst>
 </file>
@@ -623,16 +631,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E52"/>
+  <dimension ref="A2:E63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C44" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="62.33203125" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" customWidth="1"/>
+    <col min="3" max="3" width="91.33203125" customWidth="1"/>
     <col min="4" max="4" width="55.77734375" customWidth="1"/>
     <col min="5" max="5" width="45.6640625" customWidth="1"/>
   </cols>
@@ -1002,6 +1010,17 @@
       </c>
       <c r="C52" s="1" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
position of a number in infinite array and renamed Readme file
</commit_message>
<xml_diff>
--- a/ZSolved Problems.xlsx
+++ b/ZSolved Problems.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
   <si>
     <t>PROBLEM SOLVED</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>Find first and last occurrence of the number in an array</t>
+  </si>
+  <si>
+    <t>Find posistion of an element in a sorted array of infinite numbers</t>
   </si>
 </sst>
 </file>
@@ -631,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E63"/>
+  <dimension ref="A2:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C44" sqref="A1:XFD1048576"/>
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,8 +1022,13 @@
       <c r="B63" t="s">
         <v>91</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="1" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1064,8 +1072,9 @@
     <hyperlink ref="C51" r:id="rId37"/>
     <hyperlink ref="C48" r:id="rId38"/>
     <hyperlink ref="C52" r:id="rId39"/>
+    <hyperlink ref="C63" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId40"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Find in mountain array hard question
</commit_message>
<xml_diff>
--- a/ZSolved Problems.xlsx
+++ b/ZSolved Problems.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="96">
   <si>
     <t>PROBLEM SOLVED</t>
   </si>
@@ -303,6 +303,15 @@
   </si>
   <si>
     <t>Find posistion of an element in a sorted array of infinite numbers</t>
+  </si>
+  <si>
+    <t>Peak Index in Mountain Array</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/find-peak-element/</t>
+  </si>
+  <si>
+    <t>Search on GFG || Kunal Kushwaha Binary Search Four Hour Video</t>
   </si>
 </sst>
 </file>
@@ -634,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E64"/>
+  <dimension ref="A2:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1029,6 +1038,17 @@
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>92</v>
+      </c>
+      <c r="C64" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>93</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1073,8 +1093,9 @@
     <hyperlink ref="C48" r:id="rId38"/>
     <hyperlink ref="C52" r:id="rId39"/>
     <hyperlink ref="C63" r:id="rId40"/>
+    <hyperlink ref="C65" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>